<commit_message>
File Import and Data Reading ✔️
</commit_message>
<xml_diff>
--- a/uploads/Employee_Data.xlsx
+++ b/uploads/Employee_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal Work\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63991701-F212-4588-ADF4-41A7773027C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02614B57-3874-4B58-94A1-1C8C10A580E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{558040A5-EDA5-461F-8C90-BD78AFE316FF}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t xml:space="preserve">Name </t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>asa@gmail.com</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,35 +438,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>